<commit_message>
fix problem wrong index in glob
</commit_message>
<xml_diff>
--- a/data/opt_solomon/all_25.xlsx
+++ b/data/opt_solomon/all_25.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payakorn_sak\.julia\dev\VehicleRoutingProblems\data\opt_solomon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF8CF295-56D2-43DE-9909-77E38AEBAB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41215323-9AE0-411F-A43D-9EA25E0CA0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2385" windowWidth="24240" windowHeight="13140"/>
+    <workbookView xWindow="-24120" yWindow="2385" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_25" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
   <si>
     <t>Problem</t>
   </si>
@@ -206,12 +206,15 @@
   </si>
   <si>
     <t>RC208</t>
+  </si>
+  <si>
+    <t>Our_NV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1045,11 +1048,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,11 +1076,17 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
       <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>62</v>
       </c>
       <c r="M1" t="s">
         <v>4</v>
@@ -1102,14 +1111,17 @@
       <c r="F2">
         <v>191.9</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
       <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
         <v>191.3</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
       </c>
       <c r="M2">
         <v>191.3</v>
@@ -1134,14 +1146,17 @@
       <c r="F3">
         <v>190.8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
       <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="K3">
         <v>190.3</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
       </c>
       <c r="M3">
         <v>190.3</v>
@@ -1166,14 +1181,17 @@
       <c r="F4">
         <v>190.8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
       <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
         <v>190.3</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
       </c>
       <c r="M4">
         <v>190.3</v>
@@ -1198,14 +1216,17 @@
       <c r="F5">
         <v>187.5</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
         <v>9</v>
       </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
       <c r="J5">
-        <v>3</v>
-      </c>
-      <c r="K5">
         <v>186.9</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
       </c>
       <c r="M5">
         <v>186.9</v>
@@ -1230,14 +1251,17 @@
       <c r="F6">
         <v>191.9</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
         <v>10</v>
       </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
       <c r="J6">
-        <v>3</v>
-      </c>
-      <c r="K6">
         <v>191.3</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
       </c>
       <c r="M6">
         <v>191.3</v>
@@ -1262,14 +1286,17 @@
       <c r="F7">
         <v>191.9</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" t="s">
         <v>11</v>
       </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
       <c r="J7">
-        <v>3</v>
-      </c>
-      <c r="K7">
         <v>191.3</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
       </c>
       <c r="M7">
         <v>191.3</v>
@@ -1294,14 +1321,17 @@
       <c r="F8">
         <v>191.9</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8" t="s">
         <v>12</v>
       </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
       <c r="J8">
-        <v>3</v>
-      </c>
-      <c r="K8">
         <v>191.3</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
       </c>
       <c r="M8">
         <v>191.3</v>
@@ -1326,14 +1356,17 @@
       <c r="F9">
         <v>191.9</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" t="s">
         <v>13</v>
       </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
       <c r="J9">
-        <v>3</v>
-      </c>
-      <c r="K9">
         <v>191.3</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
       </c>
       <c r="M9">
         <v>191.3</v>
@@ -1358,14 +1391,17 @@
       <c r="F10">
         <v>191.9</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H10" t="s">
         <v>14</v>
       </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
       <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
         <v>191.3</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
       </c>
       <c r="M10">
         <v>191.3</v>
@@ -1390,14 +1426,17 @@
       <c r="F11">
         <v>215.6</v>
       </c>
-      <c r="I11" t="s">
+      <c r="H11" t="s">
         <v>15</v>
       </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
       <c r="J11">
-        <v>2</v>
-      </c>
-      <c r="K11">
         <v>214.7</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
       </c>
       <c r="M11">
         <v>214.7</v>
@@ -1422,14 +1461,17 @@
       <c r="F12">
         <v>215.6</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H12" t="s">
         <v>16</v>
       </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
       <c r="J12">
-        <v>2</v>
-      </c>
-      <c r="K12">
         <v>214.7</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
       </c>
       <c r="M12">
         <v>214.7</v>
@@ -1454,17 +1496,20 @@
       <c r="F13">
         <v>215.6</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" t="s">
         <v>17</v>
       </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
       <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13">
         <v>214.7</v>
       </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
       <c r="M13">
-        <v>214.7</v>
+        <v>239.4</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1486,17 +1531,20 @@
       <c r="F14">
         <v>215.4</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14" t="s">
         <v>18</v>
       </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
       <c r="J14">
-        <v>2</v>
-      </c>
-      <c r="K14">
         <v>213.1</v>
       </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
       <c r="M14">
-        <v>214.5</v>
+        <v>244.4</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1518,14 +1566,17 @@
       <c r="F15">
         <v>215.6</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H15" t="s">
         <v>19</v>
       </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
       <c r="J15">
-        <v>2</v>
-      </c>
-      <c r="K15">
         <v>214.7</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
       </c>
       <c r="M15">
         <v>214.7</v>
@@ -1550,14 +1601,17 @@
       <c r="F16">
         <v>215.6</v>
       </c>
-      <c r="I16" t="s">
+      <c r="H16" t="s">
         <v>20</v>
       </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
       <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="K16">
         <v>214.7</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
       </c>
       <c r="M16">
         <v>214.7</v>
@@ -1582,17 +1636,20 @@
       <c r="F17">
         <v>274.8</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H17" t="s">
         <v>21</v>
       </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
       <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="K17">
         <v>214.5</v>
       </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
       <c r="M17">
-        <v>274.10000000000002</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1614,14 +1671,17 @@
       <c r="F18">
         <v>229.9</v>
       </c>
-      <c r="I18" t="s">
+      <c r="H18" t="s">
         <v>22</v>
       </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
       <c r="J18">
-        <v>2</v>
-      </c>
-      <c r="K18">
         <v>214.5</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
       </c>
       <c r="M18">
         <v>229.1</v>
@@ -1646,14 +1706,17 @@
       <c r="F19">
         <v>618.4</v>
       </c>
-      <c r="I19" t="s">
+      <c r="H19" t="s">
         <v>23</v>
       </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
       <c r="J19">
+        <v>617.1</v>
+      </c>
+      <c r="L19">
         <v>8</v>
-      </c>
-      <c r="K19">
-        <v>617.1</v>
       </c>
       <c r="M19">
         <v>617.1</v>
@@ -1678,14 +1741,17 @@
       <c r="F20">
         <v>548.20000000000005</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H20" t="s">
         <v>24</v>
       </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
       <c r="J20">
+        <v>547.1</v>
+      </c>
+      <c r="L20">
         <v>7</v>
-      </c>
-      <c r="K20">
-        <v>547.1</v>
       </c>
       <c r="M20">
         <v>547.1</v>
@@ -1710,14 +1776,17 @@
       <c r="F21">
         <v>455.7</v>
       </c>
-      <c r="I21" t="s">
-        <v>25</v>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
       </c>
       <c r="J21">
+        <v>454.6</v>
+      </c>
+      <c r="L21">
         <v>5</v>
-      </c>
-      <c r="K21">
-        <v>454.6</v>
       </c>
       <c r="M21">
         <v>454.6</v>
@@ -1742,14 +1811,17 @@
       <c r="F22">
         <v>418</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H22" t="s">
         <v>26</v>
       </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
       <c r="J22">
+        <v>416.9</v>
+      </c>
+      <c r="L22">
         <v>4</v>
-      </c>
-      <c r="K22">
-        <v>416.9</v>
       </c>
       <c r="M22">
         <v>416.9</v>
@@ -1774,14 +1846,17 @@
       <c r="F23">
         <v>531.6</v>
       </c>
-      <c r="I23" t="s">
+      <c r="H23" t="s">
         <v>27</v>
       </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
       <c r="J23">
+        <v>530.5</v>
+      </c>
+      <c r="L23">
         <v>6</v>
-      </c>
-      <c r="K23">
-        <v>530.5</v>
       </c>
       <c r="M23">
         <v>530.5</v>
@@ -1806,17 +1881,20 @@
       <c r="F24">
         <v>466.5</v>
       </c>
-      <c r="I24" t="s">
+      <c r="H24" t="s">
         <v>28</v>
       </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
       <c r="J24">
-        <v>3</v>
-      </c>
-      <c r="K24">
         <v>465.4</v>
       </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
       <c r="M24">
-        <v>465.5</v>
+        <v>465.4</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1838,14 +1916,17 @@
       <c r="F25">
         <v>431.9</v>
       </c>
-      <c r="I25" t="s">
+      <c r="H25" t="s">
         <v>29</v>
       </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
       <c r="J25">
-        <v>4</v>
-      </c>
-      <c r="K25">
         <v>424.3</v>
+      </c>
+      <c r="L25">
+        <v>5</v>
       </c>
       <c r="M25">
         <v>430.8</v>
@@ -1870,14 +1951,17 @@
       <c r="F26">
         <v>398.3</v>
       </c>
-      <c r="I26" t="s">
+      <c r="H26" t="s">
         <v>30</v>
       </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
       <c r="J26">
+        <v>397.3</v>
+      </c>
+      <c r="L26">
         <v>4</v>
-      </c>
-      <c r="K26">
-        <v>397.3</v>
       </c>
       <c r="M26">
         <v>397.3</v>
@@ -1902,14 +1986,17 @@
       <c r="F27">
         <v>442.7</v>
       </c>
-      <c r="I27" t="s">
+      <c r="H27" t="s">
         <v>31</v>
       </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
       <c r="J27">
+        <v>441.3</v>
+      </c>
+      <c r="L27">
         <v>5</v>
-      </c>
-      <c r="K27">
-        <v>441.3</v>
       </c>
       <c r="M27">
         <v>441.3</v>
@@ -1934,17 +2021,20 @@
       <c r="F28">
         <v>445.2</v>
       </c>
-      <c r="I28" t="s">
+      <c r="H28" t="s">
         <v>32</v>
       </c>
+      <c r="I28">
+        <v>4</v>
+      </c>
       <c r="J28">
-        <v>4</v>
-      </c>
-      <c r="K28">
         <v>444.1</v>
       </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
       <c r="M28">
-        <v>444.2</v>
+        <v>444.1</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1966,17 +2056,20 @@
       <c r="F29">
         <v>429.7</v>
       </c>
-      <c r="I29" t="s">
+      <c r="H29" t="s">
         <v>33</v>
       </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
       <c r="J29">
-        <v>5</v>
-      </c>
-      <c r="K29">
         <v>428.8</v>
       </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
       <c r="M29">
-        <v>428.9</v>
+        <v>428.8</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1998,14 +2091,17 @@
       <c r="F30">
         <v>394.2</v>
       </c>
-      <c r="I30" t="s">
+      <c r="H30" t="s">
         <v>34</v>
       </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
       <c r="J30">
+        <v>393</v>
+      </c>
+      <c r="L30">
         <v>4</v>
-      </c>
-      <c r="K30">
-        <v>393</v>
       </c>
       <c r="M30">
         <v>393</v>
@@ -2030,14 +2126,17 @@
       <c r="F31">
         <v>464.4</v>
       </c>
-      <c r="I31" t="s">
+      <c r="H31" t="s">
         <v>35</v>
       </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
       <c r="J31">
+        <v>463.3</v>
+      </c>
+      <c r="L31">
         <v>4</v>
-      </c>
-      <c r="K31">
-        <v>463.3</v>
       </c>
       <c r="M31">
         <v>463.3</v>
@@ -2062,14 +2161,17 @@
       <c r="F32">
         <v>411.5</v>
       </c>
-      <c r="I32" t="s">
+      <c r="H32" t="s">
         <v>36</v>
       </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
       <c r="J32">
+        <v>410.5</v>
+      </c>
+      <c r="L32">
         <v>4</v>
-      </c>
-      <c r="K32">
-        <v>410.5</v>
       </c>
       <c r="M32">
         <v>410.5</v>
@@ -2094,17 +2196,20 @@
       <c r="F33">
         <v>392.4</v>
       </c>
-      <c r="I33" t="s">
+      <c r="H33" t="s">
         <v>37</v>
       </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
       <c r="J33">
-        <v>3</v>
-      </c>
-      <c r="K33">
         <v>391.4</v>
       </c>
+      <c r="L33">
+        <v>3</v>
+      </c>
       <c r="M33">
-        <v>391.4</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2126,17 +2231,20 @@
       <c r="F34">
         <v>355.9</v>
       </c>
-      <c r="I34" t="s">
+      <c r="H34" t="s">
         <v>38</v>
       </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
       <c r="J34">
-        <v>2</v>
-      </c>
-      <c r="K34">
         <v>355</v>
       </c>
+      <c r="L34">
+        <v>2</v>
+      </c>
       <c r="M34">
-        <v>355.1</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2158,17 +2266,20 @@
       <c r="F35">
         <v>394.1</v>
       </c>
-      <c r="I35" t="s">
+      <c r="H35" t="s">
         <v>39</v>
       </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
       <c r="J35">
-        <v>3</v>
-      </c>
-      <c r="K35">
         <v>393</v>
       </c>
+      <c r="L35">
+        <v>3</v>
+      </c>
       <c r="M35">
-        <v>393.1</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2190,17 +2301,20 @@
       <c r="F36">
         <v>375.5</v>
       </c>
-      <c r="I36" t="s">
+      <c r="H36" t="s">
         <v>40</v>
       </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
       <c r="J36">
-        <v>3</v>
-      </c>
-      <c r="K36">
         <v>374.4</v>
       </c>
+      <c r="L36">
+        <v>3</v>
+      </c>
       <c r="M36">
-        <v>374.5</v>
+        <v>374.4</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2222,17 +2336,20 @@
       <c r="F37">
         <v>362.7</v>
       </c>
-      <c r="I37" t="s">
+      <c r="H37" t="s">
         <v>41</v>
       </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
       <c r="J37">
-        <v>3</v>
-      </c>
-      <c r="K37">
         <v>361.6</v>
       </c>
+      <c r="L37">
+        <v>2</v>
+      </c>
       <c r="M37">
-        <v>361.6</v>
+        <v>372.2</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2254,17 +2371,20 @@
       <c r="F38">
         <v>329.4</v>
       </c>
-      <c r="I38" t="s">
+      <c r="H38" t="s">
         <v>42</v>
       </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
       <c r="J38">
+        <v>328.2</v>
+      </c>
+      <c r="L38">
         <v>1</v>
       </c>
-      <c r="K38">
-        <v>328.2</v>
-      </c>
       <c r="M38">
-        <v>328.2</v>
+        <v>345.1</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2286,17 +2406,20 @@
       <c r="F39">
         <v>371.6</v>
       </c>
-      <c r="I39" t="s">
+      <c r="H39" t="s">
         <v>43</v>
       </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
       <c r="J39">
-        <v>2</v>
-      </c>
-      <c r="K39">
         <v>370.7</v>
       </c>
+      <c r="L39">
+        <v>3</v>
+      </c>
       <c r="M39">
-        <v>370.8</v>
+        <v>380.9</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2318,14 +2441,17 @@
       <c r="F40">
         <v>405.5</v>
       </c>
-      <c r="I40" t="s">
+      <c r="H40" t="s">
         <v>44</v>
       </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
       <c r="J40">
-        <v>3</v>
-      </c>
-      <c r="K40">
         <v>404.6</v>
+      </c>
+      <c r="L40">
+        <v>3</v>
       </c>
       <c r="M40">
         <v>404.6</v>
@@ -2350,17 +2476,20 @@
       <c r="F41">
         <v>352</v>
       </c>
-      <c r="I41" t="s">
+      <c r="H41" t="s">
         <v>45</v>
       </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
       <c r="J41">
-        <v>2</v>
-      </c>
-      <c r="K41">
         <v>350.9</v>
       </c>
+      <c r="L41">
+        <v>3</v>
+      </c>
       <c r="M41">
-        <v>350.9</v>
+        <v>379.4</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2382,17 +2511,20 @@
       <c r="F42">
         <v>462.2</v>
       </c>
-      <c r="I42" t="s">
+      <c r="H42" t="s">
         <v>46</v>
       </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
       <c r="J42">
-        <v>4</v>
-      </c>
-      <c r="K42">
         <v>461.1</v>
       </c>
+      <c r="L42">
+        <v>5</v>
+      </c>
       <c r="M42">
-        <v>461.1</v>
+        <v>515.6</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2414,17 +2546,20 @@
       <c r="F43">
         <v>352.8</v>
       </c>
-      <c r="I43" t="s">
+      <c r="H43" t="s">
         <v>47</v>
       </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
       <c r="J43">
-        <v>3</v>
-      </c>
-      <c r="K43">
         <v>351.8</v>
       </c>
+      <c r="L43">
+        <v>3</v>
+      </c>
       <c r="M43">
-        <v>351.9</v>
+        <v>351.8</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2446,14 +2581,17 @@
       <c r="F44">
         <v>334</v>
       </c>
-      <c r="I44" t="s">
+      <c r="H44" t="s">
         <v>48</v>
       </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
       <c r="J44">
-        <v>3</v>
-      </c>
-      <c r="K44">
         <v>332.8</v>
+      </c>
+      <c r="L44">
+        <v>3</v>
       </c>
       <c r="M44">
         <v>332.8</v>
@@ -2478,14 +2616,17 @@
       <c r="F45">
         <v>307.2</v>
       </c>
-      <c r="I45" t="s">
+      <c r="H45" t="s">
         <v>49</v>
       </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
       <c r="J45">
-        <v>3</v>
-      </c>
-      <c r="K45">
         <v>306.60000000000002</v>
+      </c>
+      <c r="L45">
+        <v>3</v>
       </c>
       <c r="M45">
         <v>306.60000000000002</v>
@@ -2510,17 +2651,20 @@
       <c r="F46">
         <v>412.4</v>
       </c>
-      <c r="I46" t="s">
+      <c r="H46" t="s">
         <v>50</v>
       </c>
+      <c r="I46">
+        <v>4</v>
+      </c>
       <c r="J46">
+        <v>411.3</v>
+      </c>
+      <c r="L46">
         <v>4</v>
       </c>
-      <c r="K46">
-        <v>411.3</v>
-      </c>
       <c r="M46">
-        <v>411.3</v>
+        <v>415.1</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2542,17 +2686,20 @@
       <c r="F47">
         <v>346.6</v>
       </c>
-      <c r="I47" t="s">
+      <c r="H47" t="s">
         <v>51</v>
       </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
       <c r="J47">
-        <v>3</v>
-      </c>
-      <c r="K47">
         <v>345.5</v>
       </c>
+      <c r="L47">
+        <v>3</v>
+      </c>
       <c r="M47">
-        <v>345.6</v>
+        <v>345.5</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2574,14 +2721,17 @@
       <c r="F48">
         <v>299</v>
       </c>
-      <c r="I48" t="s">
+      <c r="H48" t="s">
         <v>52</v>
       </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
       <c r="J48">
-        <v>3</v>
-      </c>
-      <c r="K48">
         <v>298.3</v>
+      </c>
+      <c r="L48">
+        <v>3</v>
       </c>
       <c r="M48">
         <v>298.3</v>
@@ -2606,17 +2756,20 @@
       <c r="F49">
         <v>295</v>
       </c>
-      <c r="I49" t="s">
+      <c r="H49" t="s">
         <v>53</v>
       </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
       <c r="J49">
-        <v>3</v>
-      </c>
-      <c r="K49">
         <v>294.5</v>
       </c>
+      <c r="L49">
+        <v>3</v>
+      </c>
       <c r="M49">
-        <v>294.60000000000002</v>
+        <v>294.5</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2638,14 +2791,17 @@
       <c r="F50">
         <v>361.3</v>
       </c>
-      <c r="I50" t="s">
+      <c r="H50" t="s">
         <v>54</v>
       </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
       <c r="J50">
-        <v>3</v>
-      </c>
-      <c r="K50">
         <v>360.2</v>
+      </c>
+      <c r="L50">
+        <v>3</v>
       </c>
       <c r="M50">
         <v>360.2</v>
@@ -2670,17 +2826,20 @@
       <c r="F51">
         <v>338.9</v>
       </c>
-      <c r="I51" t="s">
+      <c r="H51" t="s">
         <v>55</v>
       </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
       <c r="J51">
-        <v>3</v>
-      </c>
-      <c r="K51">
         <v>338</v>
       </c>
+      <c r="L51">
+        <v>3</v>
+      </c>
       <c r="M51">
-        <v>338.1</v>
+        <v>338</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -2702,17 +2861,20 @@
       <c r="F52">
         <v>327.7</v>
       </c>
-      <c r="I52" t="s">
+      <c r="H52" t="s">
         <v>56</v>
       </c>
+      <c r="I52">
+        <v>3</v>
+      </c>
       <c r="J52">
-        <v>3</v>
-      </c>
-      <c r="K52">
         <v>326.89999999999998</v>
       </c>
+      <c r="L52">
+        <v>3</v>
+      </c>
       <c r="M52">
-        <v>327</v>
+        <v>326.89999999999998</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -2734,17 +2896,20 @@
       <c r="F53">
         <v>300.3</v>
       </c>
-      <c r="I53" t="s">
+      <c r="H53" t="s">
         <v>57</v>
       </c>
+      <c r="I53">
+        <v>3</v>
+      </c>
       <c r="J53">
-        <v>3</v>
-      </c>
-      <c r="K53">
         <v>299.7</v>
       </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
       <c r="M53">
-        <v>299.8</v>
+        <v>458</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -2766,14 +2931,17 @@
       <c r="F54">
         <v>339</v>
       </c>
-      <c r="I54" t="s">
+      <c r="H54" t="s">
         <v>58</v>
       </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
       <c r="J54">
-        <v>3</v>
-      </c>
-      <c r="K54">
         <v>338</v>
+      </c>
+      <c r="L54">
+        <v>3</v>
       </c>
       <c r="M54">
         <v>338</v>
@@ -2798,17 +2966,20 @@
       <c r="F55">
         <v>325.2</v>
       </c>
-      <c r="I55" t="s">
+      <c r="H55" t="s">
         <v>59</v>
       </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
       <c r="J55">
-        <v>3</v>
-      </c>
-      <c r="K55">
         <v>324</v>
       </c>
+      <c r="L55">
+        <v>2</v>
+      </c>
       <c r="M55">
-        <v>324.10000000000002</v>
+        <v>369.1</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -2830,14 +3001,17 @@
       <c r="F56">
         <v>299</v>
       </c>
-      <c r="I56" t="s">
+      <c r="H56" t="s">
         <v>60</v>
       </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
       <c r="J56">
-        <v>3</v>
-      </c>
-      <c r="K56">
         <v>298.3</v>
+      </c>
+      <c r="L56">
+        <v>3</v>
       </c>
       <c r="M56">
         <v>298.3</v>
@@ -2862,14 +3036,17 @@
       <c r="F57">
         <v>269.60000000000002</v>
       </c>
-      <c r="I57" t="s">
+      <c r="H57" t="s">
         <v>61</v>
       </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
       <c r="J57">
-        <v>2</v>
-      </c>
-      <c r="K57">
         <v>269.10000000000002</v>
+      </c>
+      <c r="L57">
+        <v>2</v>
       </c>
       <c r="M57">
         <v>269.10000000000002</v>

</xml_diff>